<commit_message>
Official BMI recalculation, updated presentation with new demographics table
</commit_message>
<xml_diff>
--- a/Project2/Reports/TableOverallCharacteristics_formatted.xlsx
+++ b/Project2/Reports/TableOverallCharacteristics_formatted.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="TableOverallCharacteristics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcCompleted="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -33,13 +33,13 @@
     <t>Valve surgery</t>
   </si>
   <si>
-    <t>6174 (23.28)</t>
+    <t>5612 (21.16)</t>
   </si>
   <si>
     <t>CABG surgery</t>
   </si>
   <si>
-    <t>21589 (81.41)</t>
+    <t>21459 (80.92)</t>
   </si>
   <si>
     <t>ASA (n (%))</t>
@@ -51,25 +51,25 @@
     <t>21 (0.08)</t>
   </si>
   <si>
-    <t>1082 (4.08)</t>
-  </si>
-  <si>
-    <t>5020 (18.93)</t>
-  </si>
-  <si>
-    <t>18981 (71.58)</t>
+    <t>1115 (4.2)</t>
+  </si>
+  <si>
+    <t>5161 (19.46)</t>
+  </si>
+  <si>
+    <t>19504 (73.54)</t>
   </si>
   <si>
     <t>5 = near death</t>
   </si>
   <si>
-    <t>54 (0.2)</t>
+    <t>55 (0.21)</t>
   </si>
   <si>
     <t>Missing</t>
   </si>
   <si>
-    <t>1360 (5.13)</t>
+    <t>664 (2.5)</t>
   </si>
   <si>
     <t>BMI (median (IQR))</t>
@@ -90,13 +90,13 @@
     <t>4 (0.73)</t>
   </si>
   <si>
-    <t>13591 (51.25)</t>
+    <t>13241 (49.93)</t>
   </si>
   <si>
     <t>30 day mortality (n (%))</t>
   </si>
   <si>
-    <t>787 (2.97)</t>
+    <t>835 (3.15)</t>
   </si>
 </sst>
 </file>
@@ -252,7 +252,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,20 +432,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -571,13 +559,11 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -586,28 +572,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -658,33 +622,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1014,138 +969,137 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>26518</v>
+      <c r="B2" s="2">
+        <v>26520</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Collapsed ASA categories, started changing table to only get expected death rate for pd 39
</commit_message>
<xml_diff>
--- a/Project2/Reports/TableOverallCharacteristics_formatted.xlsx
+++ b/Project2/Reports/TableOverallCharacteristics_formatted.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Hospitals (n)</t>
   </si>
@@ -33,37 +33,28 @@
     <t>Valve surgery</t>
   </si>
   <si>
-    <t>5612 (21.16)</t>
+    <t>5610 (21.16)</t>
   </si>
   <si>
     <t>CABG surgery</t>
   </si>
   <si>
-    <t>21459 (80.92)</t>
+    <t>21457 (80.91)</t>
   </si>
   <si>
     <t>ASA (n (%))</t>
   </si>
   <si>
-    <t>1 = good health</t>
-  </si>
-  <si>
-    <t>21 (0.08)</t>
-  </si>
-  <si>
-    <t>1115 (4.2)</t>
-  </si>
-  <si>
-    <t>5161 (19.46)</t>
-  </si>
-  <si>
-    <t>19504 (73.54)</t>
-  </si>
-  <si>
-    <t>5 = near death</t>
-  </si>
-  <si>
-    <t>55 (0.21)</t>
+    <t>3 or less</t>
+  </si>
+  <si>
+    <t>6296 (23.74)</t>
+  </si>
+  <si>
+    <t>4 or greater</t>
+  </si>
+  <si>
+    <t>19558 (73.75)</t>
   </si>
   <si>
     <t>Missing</t>
@@ -90,13 +81,13 @@
     <t>4 (0.73)</t>
   </si>
   <si>
-    <t>13241 (49.93)</t>
+    <t>13239 (49.92)</t>
   </si>
   <si>
     <t>30 day mortality (n (%))</t>
   </si>
   <si>
-    <t>835 (3.15)</t>
+    <t>834 (3.15)</t>
   </si>
 </sst>
 </file>
@@ -549,16 +540,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -567,10 +551,21 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -627,19 +622,19 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -961,62 +956,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="6">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>26520</v>
+      <c r="B2" s="6">
+        <v>26518</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1024,83 +1019,59 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>2</v>
+      <c r="A8" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>4</v>
+      <c r="A10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="13" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="14" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B14" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added columns to hospital table, worked on report
</commit_message>
<xml_diff>
--- a/Project2/Reports/TableOverallCharacteristics_formatted.xlsx
+++ b/Project2/Reports/TableOverallCharacteristics_formatted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4980" windowHeight="830"/>
   </bookViews>
   <sheets>
     <sheet name="TableOverallCharacteristics" sheetId="1" r:id="rId1"/>
@@ -63,10 +63,10 @@
     <t>664 (2.5)</t>
   </si>
   <si>
-    <t>BMI (median (IQR))</t>
-  </si>
-  <si>
-    <t>28.66 (5.05)</t>
+    <t>BMI (mean (SD))</t>
+  </si>
+  <si>
+    <t>28.64 (3.78)</t>
   </si>
   <si>
     <t>Missing (n (%))</t>
@@ -75,10 +75,10 @@
     <t>702 (2.65)</t>
   </si>
   <si>
-    <t>Albumin (median (IQR))</t>
-  </si>
-  <si>
-    <t>4 (0.73)</t>
+    <t>Albumin (mean (SD))</t>
+  </si>
+  <si>
+    <t>4.02 (0.55)</t>
   </si>
   <si>
     <t>13239 (49.92)</t>
@@ -540,9 +540,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -551,21 +558,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -622,17 +618,17 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
@@ -959,118 +955,118 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>26518</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>